<commit_message>
Putting up my srtuff for the first time
</commit_message>
<xml_diff>
--- a/RollCarCode/ME 107 Rollcar Component Masses.xlsx
+++ b/RollCarCode/ME 107 Rollcar Component Masses.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pcarl\Documents\College Things\ME 107\Roll Car\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pcarl\Documents\College Things\ME 107\Roll Car\Github Code Repository\RollCarCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{C34BA822-00A3-440F-9576-3108F3CD5EBB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="8910"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="8910" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -80,7 +81,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -425,11 +426,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -526,6 +527,10 @@
       <c r="B8">
         <v>278.7</v>
       </c>
+      <c r="D8">
+        <f>B11+B10+B7+B2</f>
+        <v>2458.1999999999998</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">

</xml_diff>

<commit_message>
IDK what is diff, just need to commit stuff
</commit_message>
<xml_diff>
--- a/RollCarCode/ME 107 Rollcar Component Masses.xlsx
+++ b/RollCarCode/ME 107 Rollcar Component Masses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pcarl\Documents\College Things\ME 107\Roll Car\Github Code Repository\RollCarCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{C34BA822-00A3-440F-9576-3108F3CD5EBB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{CDB71747-19A0-4DB9-882D-9B8F7D9F099C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="8910" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Component name</t>
   </si>
@@ -76,6 +76,12 @@
   </si>
   <si>
     <t>Acrylic</t>
+  </si>
+  <si>
+    <t>Position #</t>
+  </si>
+  <si>
+    <t>Position xval (cm)</t>
   </si>
 </sst>
 </file>
@@ -427,10 +433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -556,6 +562,140 @@
         <v>701.8</v>
       </c>
     </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>10</v>
+      </c>
+      <c r="B17">
+        <v>17.8</v>
+      </c>
+      <c r="C17">
+        <v>0.1804</v>
+      </c>
+      <c r="D17">
+        <v>9.8500000000000004E-2</v>
+      </c>
+      <c r="E17">
+        <f>C17-D17</f>
+        <v>8.1900000000000001E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>8</v>
+      </c>
+      <c r="B18">
+        <v>24.4</v>
+      </c>
+      <c r="C18">
+        <v>0.22770000000000001</v>
+      </c>
+      <c r="D18">
+        <v>0.15010000000000001</v>
+      </c>
+      <c r="E18">
+        <f t="shared" ref="E18:E23" si="0">C18-D18</f>
+        <v>7.7600000000000002E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>6</v>
+      </c>
+      <c r="B19">
+        <v>32.200000000000003</v>
+      </c>
+      <c r="C19">
+        <v>0.28539999999999999</v>
+      </c>
+      <c r="D19">
+        <v>0.1973</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="0"/>
+        <v>8.8099999999999984E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>5</v>
+      </c>
+      <c r="B20">
+        <v>36.6</v>
+      </c>
+      <c r="C20">
+        <v>0.31950000000000001</v>
+      </c>
+      <c r="D20">
+        <v>0.2321</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="0"/>
+        <v>8.7400000000000005E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>4</v>
+      </c>
+      <c r="B21">
+        <v>40.799999999999997</v>
+      </c>
+      <c r="C21">
+        <v>0.35199999999999998</v>
+      </c>
+      <c r="D21">
+        <v>0.26169999999999999</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="0"/>
+        <v>9.0299999999999991E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>2</v>
+      </c>
+      <c r="B22">
+        <v>50</v>
+      </c>
+      <c r="C22">
+        <v>0.4264</v>
+      </c>
+      <c r="D22">
+        <v>0.32729999999999998</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="0"/>
+        <v>9.9100000000000021E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>1</v>
+      </c>
+      <c r="B23">
+        <v>55</v>
+      </c>
+      <c r="C23">
+        <v>0.46839999999999998</v>
+      </c>
+      <c r="D23">
+        <v>0.35360000000000003</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="0"/>
+        <v>0.11479999999999996</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>